<commit_message>
Added complete test data
</commit_message>
<xml_diff>
--- a/src/test/java/ExternalFiles/TestData.xlsx
+++ b/src/test/java/ExternalFiles/TestData.xlsx
@@ -14,20 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>userName</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>rbrahulbarapatre@gmail.com</t>
-  </si>
-  <si>
-    <t>Ra9892338563@</t>
-  </si>
-  <si>
     <t>TC55</t>
   </si>
   <si>
@@ -53,6 +44,48 @@
   </si>
   <si>
     <t>test@rahul.com</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>https://ui.cogmento.com/</t>
+  </si>
+  <si>
+    <t>rahulscreencast9892@gmail.com</t>
+  </si>
+  <si>
+    <t>Ra987456321@</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Sumeet</t>
+  </si>
+  <si>
+    <t>Desai</t>
+  </si>
+  <si>
+    <t>sumeet.desai@gmail.com</t>
+  </si>
+  <si>
+    <t>Create a follow up activity</t>
   </si>
 </sst>
 </file>
@@ -422,84 +455,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="C7" s="2">
         <v>9895462133</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>
     <hyperlink ref="D7" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="B3" r:id="rId4"/>
+    <hyperlink ref="G3" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Excel data changes in master
</commit_message>
<xml_diff>
--- a/src/test/java/ExternalFiles/TestData.xlsx
+++ b/src/test/java/ExternalFiles/TestData.xlsx
@@ -14,20 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>userName</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>rbrahulbarapatre@gmail.com</t>
-  </si>
-  <si>
-    <t>Ra9892338563@</t>
-  </si>
-  <si>
     <t>TC55</t>
   </si>
   <si>
@@ -53,6 +44,48 @@
   </si>
   <si>
     <t>test@rahul.com</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>https://ui.cogmento.com/</t>
+  </si>
+  <si>
+    <t>rahulscreencast9892@gmail.com</t>
+  </si>
+  <si>
+    <t>Ra987456321@</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Sumeet</t>
+  </si>
+  <si>
+    <t>Desai</t>
+  </si>
+  <si>
+    <t>sumeet.desai@gmail.com</t>
+  </si>
+  <si>
+    <t>Create a follow up activity</t>
   </si>
 </sst>
 </file>
@@ -422,84 +455,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="C7" s="2">
         <v>9895462133</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>
     <hyperlink ref="D7" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="B3" r:id="rId4"/>
+    <hyperlink ref="G3" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added new files to integrate the excel file data extraction changes
</commit_message>
<xml_diff>
--- a/src/test/java/ExternalFiles/TestData.xlsx
+++ b/src/test/java/ExternalFiles/TestData.xlsx
@@ -7,7 +7,12 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Regression" sheetId="1" r:id="rId1"/>
+    <sheet name="Smoke" sheetId="2" r:id="rId2"/>
+    <sheet name="Sanity" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -458,7 +463,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,4 +581,66 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added new test case opimization code
</commit_message>
<xml_diff>
--- a/src/test/java/ExternalFiles/TestData.xlsx
+++ b/src/test/java/ExternalFiles/TestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>userName</t>
   </si>
@@ -27,30 +27,9 @@
     <t>TC55</t>
   </si>
   <si>
-    <t>TC56</t>
-  </si>
-  <si>
-    <t>Firstname</t>
-  </si>
-  <si>
     <t>lastName</t>
   </si>
   <si>
-    <t>contactNumber</t>
-  </si>
-  <si>
-    <t>Emailid</t>
-  </si>
-  <si>
-    <t>Rahul</t>
-  </si>
-  <si>
-    <t>desai</t>
-  </si>
-  <si>
-    <t>test@rahul.com</t>
-  </si>
-  <si>
     <t>url</t>
   </si>
   <si>
@@ -91,6 +70,18 @@
   </si>
   <si>
     <t>Create a follow up activity</t>
+  </si>
+  <si>
+    <t>Sumeet99</t>
+  </si>
+  <si>
+    <t>Desai99</t>
+  </si>
+  <si>
+    <t>sumeet.desai99@gmail.com</t>
+  </si>
+  <si>
+    <t>Delete</t>
   </si>
 </sst>
 </file>
@@ -463,7 +454,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,51 +476,51 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -537,7 +528,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -545,39 +536,66 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2">
-        <v>9895462133</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>9</v>
+      <c r="E7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>
-    <hyperlink ref="D7" r:id="rId2"/>
-    <hyperlink ref="C3" r:id="rId3"/>
-    <hyperlink ref="B3" r:id="rId4"/>
-    <hyperlink ref="G3" r:id="rId5"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="G3" r:id="rId4"/>
+    <hyperlink ref="A7" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="B7" r:id="rId7"/>
+    <hyperlink ref="G7" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>